<commit_message>
fixings importationo payers and rake on produciton
</commit_message>
<xml_diff>
--- a/lib/xlsx_reader/sacados_biort.xlsx
+++ b/lib/xlsx_reader/sacados_biort.xlsx
@@ -30,14 +30,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="217" uniqueCount="184">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="209" uniqueCount="179">
   <si>
     <t>ID</t>
   </si>
   <si>
-    <t>CEDENTE</t>
-  </si>
-  <si>
     <t>CPF/CNPJ CEDENTE</t>
   </si>
   <si>
@@ -512,21 +509,6 @@
     <t>11+42278423</t>
   </si>
   <si>
-    <t>NOME</t>
-  </si>
-  <si>
-    <t>CPF/CNPJ</t>
-  </si>
-  <si>
-    <t>ENDEREÇO</t>
-  </si>
-  <si>
-    <t>CIDADE</t>
-  </si>
-  <si>
-    <t>TELEFONE</t>
-  </si>
-  <si>
     <t>RELATÓRIO DE CADASTRO DE SACADOS - Data Emissão: 20/02/2018</t>
   </si>
   <si>
@@ -582,6 +564,9 @@
   </si>
   <si>
     <t>11+21462682</t>
+  </si>
+  <si>
+    <t>Sacado</t>
   </si>
 </sst>
 </file>
@@ -846,11 +831,11 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="17"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="Accent 1 1" xfId="1"/>
@@ -1337,8 +1322,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -1351,34 +1336,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="16">
-      <c r="A1" s="10" t="s">
-        <v>165</v>
+      <c r="A1" s="9" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="16">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="11">
         <v>0</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="E2" s="9" t="s">
+      <c r="B2" s="11">
+        <v>1</v>
+      </c>
+      <c r="C2" s="11">
+        <v>2</v>
+      </c>
+      <c r="D2" s="11">
+        <v>3</v>
+      </c>
+      <c r="E2" s="11">
         <v>4</v>
       </c>
-      <c r="F2" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="G2" s="9" t="s">
+      <c r="F2" s="11">
+        <v>5</v>
+      </c>
+      <c r="G2" s="11">
         <v>6</v>
       </c>
-      <c r="H2" s="9" t="s">
-        <v>164</v>
+      <c r="H2" s="11">
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1386,25 +1371,25 @@
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1412,23 +1397,23 @@
         <v>445</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>11</v>
-      </c>
       <c r="F4" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1436,19 +1421,19 @@
         <v>423</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>18</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="8"/>
@@ -1458,23 +1443,23 @@
         <v>339</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="F6" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1482,23 +1467,23 @@
         <v>98</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="F7" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1506,23 +1491,23 @@
         <v>449</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>32</v>
-      </c>
       <c r="F8" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1530,25 +1515,25 @@
         <v>407</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="D9" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="F9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="4" t="s">
+      <c r="H9" s="7" t="s">
         <v>38</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1556,19 +1541,19 @@
         <v>156</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="E10" s="4">
         <v>58082057</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="8"/>
@@ -1578,19 +1563,19 @@
         <v>189</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>47</v>
-      </c>
       <c r="F11" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="8"/>
@@ -1600,19 +1585,19 @@
         <v>181</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="D12" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>50</v>
       </c>
       <c r="E12" s="4">
         <v>1323020</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="8"/>
@@ -1622,19 +1607,19 @@
         <v>442</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="D13" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="E13" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>54</v>
-      </c>
       <c r="F13" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G13" s="6"/>
       <c r="H13" s="8"/>
@@ -1644,19 +1629,19 @@
         <v>164</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="D14" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>58</v>
-      </c>
       <c r="F14" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="8"/>
@@ -1666,19 +1651,19 @@
         <v>117</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="D15" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="E15" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E15" s="4" t="s">
-        <v>62</v>
-      </c>
       <c r="F15" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="8"/>
@@ -1688,23 +1673,23 @@
         <v>96</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="D16" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="E16" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="F16" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>67</v>
       </c>
       <c r="G16" s="6"/>
       <c r="H16" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1712,19 +1697,19 @@
         <v>340</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="D17" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="E17" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>72</v>
-      </c>
       <c r="F17" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="8"/>
@@ -1734,19 +1719,19 @@
         <v>187</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="D18" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>75</v>
       </c>
       <c r="E18" s="4">
         <v>5673050</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G18" s="6"/>
       <c r="H18" s="8"/>
@@ -1756,19 +1741,19 @@
         <v>441</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="D19" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="E19" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="E19" s="4" t="s">
-        <v>79</v>
-      </c>
       <c r="F19" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G19" s="6"/>
       <c r="H19" s="8"/>
@@ -1778,19 +1763,19 @@
         <v>180</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="D20" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="E20" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>83</v>
-      </c>
       <c r="F20" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G20" s="6"/>
       <c r="H20" s="8"/>
@@ -1800,23 +1785,23 @@
         <v>379</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="D21" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="E21" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="E21" s="4" t="s">
-        <v>87</v>
-      </c>
       <c r="F21" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G21" s="6"/>
       <c r="H21" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -1824,23 +1809,23 @@
         <v>90</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="D22" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="E22" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="E22" s="4" t="s">
-        <v>92</v>
-      </c>
       <c r="F22" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G22" s="6"/>
       <c r="H22" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -1848,23 +1833,23 @@
         <v>408</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="D23" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="E23" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E23" s="4" t="s">
-        <v>97</v>
-      </c>
       <c r="F23" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G23" s="6"/>
       <c r="H23" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1872,25 +1857,25 @@
         <v>478</v>
       </c>
       <c r="B24" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="D24" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="E24" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="F24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="F24" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G24" s="4" t="s">
+      <c r="H24" s="7" t="s">
         <v>103</v>
-      </c>
-      <c r="H24" s="7" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1898,19 +1883,19 @@
         <v>479</v>
       </c>
       <c r="B25" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="D25" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="E25" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="E25" s="4" t="s">
-        <v>108</v>
-      </c>
       <c r="F25" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G25" s="6"/>
       <c r="H25" s="8"/>
@@ -1920,19 +1905,19 @@
         <v>383</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="D26" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="E26" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="E26" s="4" t="s">
-        <v>112</v>
-      </c>
       <c r="F26" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G26" s="6"/>
       <c r="H26" s="8"/>
@@ -1942,19 +1927,19 @@
         <v>438</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="D27" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="E27" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="E27" s="4" t="s">
-        <v>116</v>
-      </c>
       <c r="F27" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G27" s="6"/>
       <c r="H27" s="8"/>
@@ -1964,23 +1949,23 @@
         <v>188</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="D28" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="E28" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="F28" s="5" t="s">
         <v>120</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>121</v>
       </c>
       <c r="G28" s="6"/>
       <c r="H28" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1988,22 +1973,22 @@
         <v>480</v>
       </c>
       <c r="B29" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="D29" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="E29" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="F29" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G29" s="4" t="s">
         <v>126</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>127</v>
       </c>
       <c r="H29" s="8"/>
     </row>
@@ -2012,23 +1997,23 @@
         <v>467</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="D30" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="E30" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="E30" s="4" t="s">
-        <v>131</v>
-      </c>
       <c r="F30" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G30" s="6"/>
       <c r="H30" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -2036,23 +2021,23 @@
         <v>437</v>
       </c>
       <c r="B31" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="D31" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="E31" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="F31" s="5" t="s">
         <v>136</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>137</v>
       </c>
       <c r="G31" s="6"/>
       <c r="H31" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -2060,23 +2045,23 @@
         <v>380</v>
       </c>
       <c r="B32" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="D32" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="E32" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="E32" s="4" t="s">
-        <v>142</v>
-      </c>
       <c r="F32" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G32" s="6"/>
       <c r="H32" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -2084,23 +2069,23 @@
         <v>389</v>
       </c>
       <c r="B33" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="D33" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="E33" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="E33" s="4" t="s">
-        <v>147</v>
-      </c>
       <c r="F33" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G33" s="6"/>
       <c r="H33" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -2108,23 +2093,23 @@
         <v>139</v>
       </c>
       <c r="B34" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="D34" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="E34" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="E34" s="4" t="s">
-        <v>152</v>
-      </c>
       <c r="F34" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G34" s="6"/>
       <c r="H34" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -2132,23 +2117,23 @@
         <v>390</v>
       </c>
       <c r="B35" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C35" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="D35" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="E35" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="E35" s="4" t="s">
+      <c r="F35" s="5" t="s">
         <v>157</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>158</v>
       </c>
       <c r="G35" s="6"/>
       <c r="H35" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -2156,23 +2141,23 @@
         <v>435</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G36" s="6"/>
       <c r="H36" s="7" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -2180,23 +2165,23 @@
         <v>456</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G37" s="6"/>
       <c r="H37" s="7" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -2204,19 +2189,19 @@
         <v>457</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G38" s="6"/>
       <c r="H38" s="7"/>
@@ -2226,23 +2211,23 @@
         <v>97</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G39" s="6"/>
       <c r="H39" s="7" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -2255,7 +2240,7 @@
       <c r="A42"/>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="11"/>
+      <c r="A43" s="10"/>
     </row>
     <row r="44" spans="1:8">
       <c r="A44"/>

</xml_diff>